<commit_message>
feat(chore): [scripts/] - Migración completa de Makefile a sistema modular Node.js con documentación exhaustiva [jira:T-01]
</commit_message>
<xml_diff>
--- a/docs/traceability.xlsx
+++ b/docs/traceability.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -438,167 +438,391 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>USR-001</v>
+        <v>USR-01</v>
       </c>
       <c r="B2" t="str">
-        <v>OAuth 2.0 Google/MS + JWT</v>
+        <v>Autenticación de usuarios con OAuth</v>
       </c>
       <c r="C2" t="str">
-        <v>T-02</v>
+        <v>T-01</v>
       </c>
       <c r="D2" t="str">
-        <v>OAuth 2.0 + JWT con Roles y Refresh Token</v>
+        <v>Configuración de CI/CD</v>
       </c>
       <c r="E2" t="str">
-        <v>cypress/e2e/auth.cy.ts</v>
+        <v>tests/auth/oauth.test.js</v>
       </c>
       <c r="F2" t="str">
-        <v>OAuth login flow</v>
+        <v/>
       </c>
       <c r="G2" t="str">
-        <v>Planned</v>
+        <v>Completado</v>
       </c>
       <c r="H2" t="str">
-        <v>R0.WP2</v>
+        <v>R0.0</v>
       </c>
       <c r="I2" t="str">
-        <v>ADR-009</v>
+        <v/>
       </c>
       <c r="J2" t="str">
-        <v>2025-06-25</v>
+        <v>2025-06-29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>GEN-001</v>
+        <v>USR-02</v>
       </c>
       <c r="B3" t="str">
-        <v>Prompt libre generation</v>
+        <v>Gestión de perfiles de usuario</v>
       </c>
       <c r="C3" t="str">
-        <v>T-05</v>
+        <v>T-02</v>
       </c>
       <c r="D3" t="str">
-        <v>Planner Service (/plan)</v>
+        <v>Implementación de autenticación</v>
       </c>
       <c r="E3" t="str">
-        <v>tests/api/planner.test.ts</v>
+        <v>tests/api/health.test.js</v>
       </c>
       <c r="F3" t="str">
-        <v>Plan generation E2E</v>
+        <v/>
       </c>
       <c r="G3" t="str">
-        <v>Planned</v>
+        <v>Completado</v>
       </c>
       <c r="H3" t="str">
-        <v>R1.WP2</v>
+        <v>R0.1</v>
       </c>
       <c r="I3" t="str">
-        <v>ADR-010</v>
+        <v/>
       </c>
       <c r="J3" t="str">
-        <v>2025-06-25</v>
+        <v>2025-06-29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>EDT-001</v>
+        <v>USR-02</v>
       </c>
       <c r="B4" t="str">
-        <v>Editor MD + comandos IA</v>
+        <v>Gestión de perfiles de usuario</v>
       </c>
       <c r="C4" t="str">
-        <v>T-07</v>
+        <v>T-17</v>
       </c>
       <c r="D4" t="str">
-        <v>Editor UI Core + Split View</v>
+        <v>Validación de API y gobernanza</v>
       </c>
       <c r="E4" t="str">
-        <v>cypress/e2e/editor.cy.ts</v>
+        <v>tests/components/editor.test.js</v>
       </c>
       <c r="F4" t="str">
-        <v>Monaco editor integration</v>
+        <v/>
       </c>
       <c r="G4" t="str">
-        <v>Planned</v>
+        <v>En Progreso</v>
       </c>
       <c r="H4" t="str">
-        <v>R2.WP1</v>
+        <v>R0.1</v>
       </c>
       <c r="I4" t="str">
-        <v>ADR-011</v>
+        <v/>
       </c>
       <c r="J4" t="str">
-        <v>2025-06-25</v>
+        <v>2025-06-29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>PERF-001</v>
+        <v>GEN-01</v>
       </c>
       <c r="B5" t="str">
-        <v>Document generation ≤8 min</v>
+        <v>Generación de documentos con IA</v>
       </c>
       <c r="C5" t="str">
-        <v>T-20</v>
+        <v>T-17</v>
       </c>
       <c r="D5" t="str">
-        <v>Bench E2E Performance</v>
+        <v>Validación de API y gobernanza</v>
       </c>
       <c r="E5" t="str">
-        <v>tests/performance/generation.test.ts</v>
+        <v>tests/components/editor.test.js</v>
       </c>
       <c r="F5" t="str">
-        <v>End-to-end generation benchmark</v>
+        <v/>
       </c>
       <c r="G5" t="str">
-        <v>Planned</v>
+        <v>En Progreso</v>
       </c>
       <c r="H5" t="str">
-        <v>R6.WP3</v>
+        <v>R0.2</v>
       </c>
       <c r="I5" t="str">
-        <v>ADR-012</v>
+        <v/>
       </c>
       <c r="J5" t="str">
-        <v>2025-06-25</v>
+        <v>2025-06-29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>SEC-001</v>
+        <v>GEN-02</v>
       </c>
       <c r="B6" t="str">
-        <v>AES-256 at-rest encryption</v>
+        <v>Personalización de plantillas</v>
       </c>
       <c r="C6" t="str">
-        <v>T-12</v>
+        <v>T-23</v>
       </c>
       <c r="D6" t="str">
-        <v>Credential Store &amp; Crypto</v>
+        <v>Endpoint de health-check</v>
       </c>
       <c r="E6" t="str">
-        <v>tests/security/encryption.test.ts</v>
+        <v>tests/services/ai-service.test.js</v>
       </c>
       <c r="F6" t="str">
-        <v>Encryption validation</v>
+        <v/>
       </c>
       <c r="G6" t="str">
-        <v>Planned</v>
+        <v>Planificado</v>
       </c>
       <c r="H6" t="str">
-        <v>R0.WP3</v>
+        <v>R0.3</v>
       </c>
       <c r="I6" t="str">
-        <v>ADR-009</v>
+        <v/>
       </c>
       <c r="J6" t="str">
-        <v>2025-06-25</v>
+        <v>2025-06-29</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>GEN-02</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Personalización de plantillas</v>
+      </c>
+      <c r="C7" t="str">
+        <v>T-41</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Integración con OpenAI</v>
+      </c>
+      <c r="E7" t="str">
+        <v>tests/utils/encryption.test.js</v>
+      </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+      <c r="G7" t="str">
+        <v>En Progreso</v>
+      </c>
+      <c r="H7" t="str">
+        <v>R0.3</v>
+      </c>
+      <c r="I7" t="str">
+        <v/>
+      </c>
+      <c r="J7" t="str">
+        <v>2025-06-29</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>EDT-01</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Editor WYSIWYG para documentos</v>
+      </c>
+      <c r="C8" t="str">
+        <v>T-41</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Integración con OpenAI</v>
+      </c>
+      <c r="E8" t="str">
+        <v>tests/utils/encryption.test.js</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+      <c r="G8" t="str">
+        <v>En Progreso</v>
+      </c>
+      <c r="H8" t="str">
+        <v>R0.4</v>
+      </c>
+      <c r="I8" t="str">
+        <v/>
+      </c>
+      <c r="J8" t="str">
+        <v>2025-06-29</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>EDT-02</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Control de versiones de documentos</v>
+      </c>
+      <c r="C9" t="str">
+        <v>T-43</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Escaneo de dependencias</v>
+      </c>
+      <c r="E9" t="str">
+        <v>tests/e2e/document-flow.test.js</v>
+      </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+      <c r="G9" t="str">
+        <v>Planificado</v>
+      </c>
+      <c r="H9" t="str">
+        <v>R1.0</v>
+      </c>
+      <c r="I9" t="str">
+        <v/>
+      </c>
+      <c r="J9" t="str">
+        <v>2025-06-29</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>EDT-02</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Control de versiones de documentos</v>
+      </c>
+      <c r="C10" t="str">
+        <v>T-44</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Editor de documentos React</v>
+      </c>
+      <c r="E10" t="str">
+        <v>tests/auth/oauth.test.js</v>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <v>En Progreso</v>
+      </c>
+      <c r="H10" t="str">
+        <v>R1.0</v>
+      </c>
+      <c r="I10" t="str">
+        <v/>
+      </c>
+      <c r="J10" t="str">
+        <v>2025-06-29</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>PERF-01</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Tiempo de respuesta &lt; 500ms</v>
+      </c>
+      <c r="C11" t="str">
+        <v>T-44</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Editor de documentos React</v>
+      </c>
+      <c r="E11" t="str">
+        <v>tests/auth/oauth.test.js</v>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+      <c r="G11" t="str">
+        <v>Completado</v>
+      </c>
+      <c r="H11" t="str">
+        <v>R1.1</v>
+      </c>
+      <c r="I11" t="str">
+        <v/>
+      </c>
+      <c r="J11" t="str">
+        <v>2025-06-29</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>SEC-01</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Cifrado de documentos en reposo</v>
+      </c>
+      <c r="C12" t="str">
+        <v>T-01</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Configuración de CI/CD</v>
+      </c>
+      <c r="E12" t="str">
+        <v>tests/api/health.test.js</v>
+      </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
+      <c r="G12" t="str">
+        <v>Completado</v>
+      </c>
+      <c r="H12" t="str">
+        <v>R1.2</v>
+      </c>
+      <c r="I12" t="str">
+        <v/>
+      </c>
+      <c r="J12" t="str">
+        <v>2025-06-29</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>SEC-01</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Cifrado de documentos en reposo</v>
+      </c>
+      <c r="C13" t="str">
+        <v>T-02</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Implementación de autenticación</v>
+      </c>
+      <c r="E13" t="str">
+        <v>tests/components/editor.test.js</v>
+      </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+      <c r="G13" t="str">
+        <v>En Progreso</v>
+      </c>
+      <c r="H13" t="str">
+        <v>R1.2</v>
+      </c>
+      <c r="I13" t="str">
+        <v/>
+      </c>
+      <c r="J13" t="str">
+        <v>2025-06-29</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J13"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -623,7 +847,7 @@
         <v>Total Requirements</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -631,7 +855,7 @@
         <v>Total Tasks</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -639,7 +863,7 @@
         <v>Total Test Files</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -655,7 +879,7 @@
         <v>Last Generated</v>
       </c>
       <c r="B6" t="str">
-        <v>2025-06-25T19:21:13.730Z</v>
+        <v>2025-06-29T16:00:18.715Z</v>
       </c>
     </row>
   </sheetData>
@@ -688,10 +912,10 @@
         <v>Authentication</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="str">
-        <v>USR-001</v>
+        <v>USR-01</v>
       </c>
     </row>
     <row r="3">
@@ -699,10 +923,10 @@
         <v>Generation</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" t="str">
-        <v>GEN-001</v>
+        <v>GEN-01</v>
       </c>
     </row>
     <row r="4">
@@ -710,10 +934,10 @@
         <v>Editor</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="str">
-        <v>EDT-001</v>
+        <v>EDT-01</v>
       </c>
     </row>
     <row r="5">
@@ -724,7 +948,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="str">
-        <v>PERF-001</v>
+        <v>PERF-01</v>
       </c>
     </row>
     <row r="6">
@@ -732,10 +956,10 @@
         <v>Security</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="str">
-        <v>SEC-001</v>
+        <v>SEC-01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(R0.WP2): complete T-41 and T-44 task validation and marking
- Mark T-41 User API Key Management as completed (9/9 points)
- Mark T-44 Admin Panel & Config Store as completed (9/9 points)
- Complete R0.WP2 work package (27/27 points - 100%)
- Update task status to "Completado 100% - DoD Satisfied"
- Update traceability documentation

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/traceability.xlsx
+++ b/docs/traceability.xlsx
@@ -63,84 +63,84 @@
     <t/>
   </si>
   <si>
+    <t>Planificado</t>
+  </si>
+  <si>
+    <t>R0.0</t>
+  </si>
+  <si>
+    <t>2025-07-01</t>
+  </si>
+  <si>
+    <t>USR-02</t>
+  </si>
+  <si>
+    <t>Gestión de perfiles de usuario</t>
+  </si>
+  <si>
+    <t>T-02</t>
+  </si>
+  <si>
+    <t>Implementación de autenticación</t>
+  </si>
+  <si>
+    <t>tests/api/health.test.js</t>
+  </si>
+  <si>
+    <t>R0.1</t>
+  </si>
+  <si>
+    <t>T-17</t>
+  </si>
+  <si>
+    <t>Validación de API y gobernanza</t>
+  </si>
+  <si>
+    <t>tests/components/editor.test.js</t>
+  </si>
+  <si>
+    <t>Completado</t>
+  </si>
+  <si>
+    <t>GEN-01</t>
+  </si>
+  <si>
+    <t>Generación de documentos con IA</t>
+  </si>
+  <si>
+    <t>R0.2</t>
+  </si>
+  <si>
+    <t>GEN-02</t>
+  </si>
+  <si>
+    <t>Personalización de plantillas</t>
+  </si>
+  <si>
+    <t>T-23</t>
+  </si>
+  <si>
+    <t>Endpoint de health-check</t>
+  </si>
+  <si>
+    <t>tests/services/ai-service.test.js</t>
+  </si>
+  <si>
+    <t>R0.3</t>
+  </si>
+  <si>
+    <t>T-41</t>
+  </si>
+  <si>
+    <t>Integración con OpenAI</t>
+  </si>
+  <si>
+    <t>tests/utils/encryption.test.js</t>
+  </si>
+  <si>
     <t>En Progreso</t>
   </si>
   <si>
-    <t>R0.0</t>
-  </si>
-  <si>
-    <t>2025-06-30</t>
-  </si>
-  <si>
-    <t>USR-02</t>
-  </si>
-  <si>
-    <t>Gestión de perfiles de usuario</t>
-  </si>
-  <si>
-    <t>T-02</t>
-  </si>
-  <si>
-    <t>Implementación de autenticación</t>
-  </si>
-  <si>
-    <t>tests/api/health.test.js</t>
-  </si>
-  <si>
-    <t>R0.1</t>
-  </si>
-  <si>
-    <t>T-17</t>
-  </si>
-  <si>
-    <t>Validación de API y gobernanza</t>
-  </si>
-  <si>
-    <t>tests/components/editor.test.js</t>
-  </si>
-  <si>
-    <t>Planificado</t>
-  </si>
-  <si>
-    <t>GEN-01</t>
-  </si>
-  <si>
-    <t>Generación de documentos con IA</t>
-  </si>
-  <si>
-    <t>R0.2</t>
-  </si>
-  <si>
-    <t>GEN-02</t>
-  </si>
-  <si>
-    <t>Personalización de plantillas</t>
-  </si>
-  <si>
-    <t>T-23</t>
-  </si>
-  <si>
-    <t>Endpoint de health-check</t>
-  </si>
-  <si>
-    <t>tests/services/ai-service.test.js</t>
-  </si>
-  <si>
-    <t>Completado</t>
-  </si>
-  <si>
-    <t>R0.3</t>
-  </si>
-  <si>
-    <t>T-41</t>
-  </si>
-  <si>
-    <t>Integración con OpenAI</t>
-  </si>
-  <si>
-    <t>tests/utils/encryption.test.js</t>
-  </si>
-  <si>
     <t>EDT-01</t>
   </si>
   <si>
@@ -216,7 +216,7 @@
     <t>Last Generated</t>
   </si>
   <si>
-    <t>2025-06-30T16:05:59.819Z</t>
+    <t>2025-07-01T15:33:51.951Z</t>
   </si>
   <si>
     <t>Category</t>
@@ -788,7 +788,7 @@
         <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
         <v>31</v>
@@ -820,10 +820,10 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
         <v>37</v>
-      </c>
-      <c r="H6" t="s">
-        <v>38</v>
       </c>
       <c r="I6" t="s">
         <v>15</v>
@@ -840,22 +840,22 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
         <v>39</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>40</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
         <v>41</v>
       </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>28</v>
-      </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
         <v>15</v>
@@ -872,13 +872,13 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
         <v>39</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
@@ -916,7 +916,7 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H9" t="s">
         <v>50</v>
@@ -948,7 +948,7 @@
         <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
         <v>50</v>
@@ -1012,7 +1012,7 @@
         <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H12" t="s">
         <v>58</v>

</xml_diff>